<commit_message>
style: update Proyecto 330.xlsx with new data
</commit_message>
<xml_diff>
--- a/src/data/Proyecto 330.xlsx
+++ b/src/data/Proyecto 330.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="353">
   <si>
     <t>Apellido</t>
   </si>
@@ -1069,6 +1069,9 @@
   </si>
   <si>
     <t>MIRIAM</t>
+  </si>
+  <si>
+    <t>MIAGROS</t>
   </si>
 </sst>
 </file>
@@ -1472,7 +1475,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
       <c r="J2" s="5">
-        <f t="shared" ref="J2:J302" si="1">SUM(D2:H2)</f>
+        <f t="shared" ref="J2:J303" si="1">SUM(D2:H2)</f>
         <v>0</v>
       </c>
     </row>
@@ -1518,18 +1521,18 @@
         <v>0</v>
       </c>
       <c r="L4" s="7">
-        <v>301.0</v>
+        <v>302.0</v>
       </c>
       <c r="M4" s="8">
         <f>SUMIF(D:I,"&lt;&gt;0")</f>
-        <v>1430000</v>
+        <v>1440000</v>
       </c>
       <c r="N4" s="8">
         <v>9000000.0</v>
       </c>
       <c r="O4" s="9">
         <f>(N4-M4)*-1</f>
-        <v>-7570000</v>
+        <v>-7560000</v>
       </c>
     </row>
     <row r="5">
@@ -8367,33 +8370,58 @@
         <v>0</v>
       </c>
     </row>
+    <row r="303">
+      <c r="A303" s="2">
+        <v>302.0</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D303" s="3">
+        <v>10000.0</v>
+      </c>
+      <c r="E303" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F303" s="5"/>
+      <c r="G303" s="6"/>
+      <c r="H303" s="5"/>
+      <c r="I303" s="6"/>
+      <c r="J303" s="5">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="$B$1:$AG$1025">
     <sortState ref="B1:AG1025">
       <sortCondition ref="B1:B1025"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="D2:D302 F2:F302 H2:H302">
+  <conditionalFormatting sqref="D2:D303 F2:F303 H2:H303">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
       <formula>10000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D302 F2:F302 H2:H302">
+  <conditionalFormatting sqref="D2:D303 F2:F303 H2:H303">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
       <formula>5000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D302 F2:F302 H2:H302">
+  <conditionalFormatting sqref="D2:D303 F2:F303 H2:H303">
     <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J302">
+  <conditionalFormatting sqref="J2:J303">
     <cfRule type="containsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(J2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J302">
+  <conditionalFormatting sqref="J2:J303">
     <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThanOrEqual">
       <formula>5000</formula>
     </cfRule>
@@ -8417,7 +8445,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E302 G2:G302 I2:I302">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E303 G2:G303 I2:I303">
       <formula1>"Efectivo,Transferencia"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
style: center text vertically in PDF export and update row height calculations
</commit_message>
<xml_diff>
--- a/src/data/Proyecto 330.xlsx
+++ b/src/data/Proyecto 330.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="409">
   <si>
     <t>Apellido</t>
   </si>
@@ -1231,6 +1231,15 @@
   </si>
   <si>
     <t>ZAPATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZILLI </t>
+  </si>
+  <si>
+    <t>GRISELDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $10.000,00</t>
   </si>
 </sst>
 </file>
@@ -1677,14 +1686,14 @@
       </c>
       <c r="M2" s="8">
         <f>SUMIF(D:I,"&lt;&gt;0")</f>
-        <v>3383000</v>
+        <v>3663000</v>
       </c>
       <c r="N2" s="8">
         <v>9000000.0</v>
       </c>
       <c r="O2" s="9">
         <f>(N2-M2)*-1</f>
-        <v>-5617000</v>
+        <v>-5337000</v>
       </c>
     </row>
     <row r="3">
@@ -1926,15 +1935,17 @@
       <c r="C10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>36</v>
@@ -2145,13 +2156,15 @@
       <c r="E18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="G18" s="6"/>
       <c r="H18" s="5"/>
       <c r="I18" s="6"/>
       <c r="J18" s="5">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="19">
@@ -2597,15 +2610,21 @@
       <c r="C36" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="5"/>
+      <c r="D36" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E36" s="4"/>
-      <c r="F36" s="5"/>
+      <c r="F36" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="G36" s="6"/>
-      <c r="H36" s="5"/>
+      <c r="H36" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="I36" s="6"/>
       <c r="J36" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="37">
@@ -3087,13 +3106,15 @@
       <c r="E56" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F56" s="5"/>
+      <c r="F56" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="G56" s="6"/>
       <c r="H56" s="5"/>
       <c r="I56" s="6"/>
       <c r="J56" s="5">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="57">
@@ -3431,7 +3452,9 @@
       <c r="C70" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D70" s="5"/>
+      <c r="D70" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E70" s="4"/>
       <c r="F70" s="5"/>
       <c r="G70" s="6"/>
@@ -3439,7 +3462,7 @@
       <c r="I70" s="6"/>
       <c r="J70" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="71">
@@ -3452,7 +3475,9 @@
       <c r="C71" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D71" s="5"/>
+      <c r="D71" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E71" s="4"/>
       <c r="F71" s="5"/>
       <c r="G71" s="6"/>
@@ -3460,7 +3485,7 @@
       <c r="I71" s="6"/>
       <c r="J71" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="72">
@@ -3583,13 +3608,15 @@
       <c r="E76" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F76" s="5"/>
+      <c r="F76" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="G76" s="6"/>
       <c r="H76" s="5"/>
       <c r="I76" s="6"/>
       <c r="J76" s="5">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="77">
@@ -3629,13 +3656,15 @@
       <c r="E78" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F78" s="5"/>
+      <c r="F78" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="G78" s="6"/>
       <c r="H78" s="5"/>
       <c r="I78" s="6"/>
       <c r="J78" s="5">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="79">
@@ -4002,15 +4031,19 @@
       <c r="C93" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D93" s="5"/>
+      <c r="D93" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E93" s="4"/>
-      <c r="F93" s="5"/>
+      <c r="F93" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="G93" s="6"/>
       <c r="H93" s="5"/>
       <c r="I93" s="6"/>
       <c r="J93" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="94">
@@ -4179,13 +4212,15 @@
       <c r="E100" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F100" s="5"/>
+      <c r="F100" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="G100" s="6"/>
       <c r="H100" s="5"/>
       <c r="I100" s="6"/>
       <c r="J100" s="5">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="101">
@@ -4565,7 +4600,9 @@
       <c r="C116" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D116" s="5"/>
+      <c r="D116" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E116" s="4"/>
       <c r="F116" s="5"/>
       <c r="G116" s="6"/>
@@ -4573,7 +4610,7 @@
       <c r="I116" s="6"/>
       <c r="J116" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="117">
@@ -4642,7 +4679,7 @@
       <c r="E119" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F119" s="5"/>
+      <c r="F119" s="6"/>
       <c r="G119" s="6"/>
       <c r="H119" s="5"/>
       <c r="I119" s="6"/>
@@ -5993,7 +6030,9 @@
       <c r="C172" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D172" s="3"/>
+      <c r="D172" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E172" s="4"/>
       <c r="F172" s="5"/>
       <c r="G172" s="6"/>
@@ -6001,7 +6040,7 @@
       <c r="I172" s="6"/>
       <c r="J172" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="173">
@@ -6014,7 +6053,9 @@
       <c r="C173" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D173" s="5"/>
+      <c r="D173" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E173" s="4"/>
       <c r="F173" s="5"/>
       <c r="G173" s="6"/>
@@ -6022,7 +6063,7 @@
       <c r="I173" s="6"/>
       <c r="J173" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="174">
@@ -6041,13 +6082,15 @@
       <c r="E174" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F174" s="5"/>
+      <c r="F174" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="G174" s="6"/>
       <c r="H174" s="5"/>
       <c r="I174" s="6"/>
       <c r="J174" s="5">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="175">
@@ -6110,7 +6153,9 @@
       <c r="C177" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D177" s="5"/>
+      <c r="D177" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E177" s="6"/>
       <c r="F177" s="5"/>
       <c r="G177" s="6"/>
@@ -6118,7 +6163,7 @@
       <c r="I177" s="6"/>
       <c r="J177" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="178">
@@ -7795,7 +7840,9 @@
       <c r="C247" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D247" s="5"/>
+      <c r="D247" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E247" s="6"/>
       <c r="F247" s="5"/>
       <c r="G247" s="6"/>
@@ -7803,7 +7850,7 @@
       <c r="I247" s="6"/>
       <c r="J247" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="248">
@@ -8563,11 +8610,13 @@
       <c r="G279" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H279" s="5"/>
+      <c r="H279" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="I279" s="6"/>
       <c r="J279" s="5">
         <f t="shared" si="2"/>
-        <v>20000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="280">
@@ -9550,15 +9599,17 @@
       <c r="C318" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D318" s="5"/>
+      <c r="D318" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E318" s="4"/>
-      <c r="F318" s="5"/>
+      <c r="F318" s="6"/>
       <c r="G318" s="6"/>
       <c r="H318" s="5"/>
       <c r="I318" s="6"/>
       <c r="J318" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="319">
@@ -10055,7 +10106,9 @@
       <c r="C339" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="D339" s="5"/>
+      <c r="D339" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E339" s="4"/>
       <c r="F339" s="5"/>
       <c r="G339" s="6"/>
@@ -10063,7 +10116,7 @@
       <c r="I339" s="6"/>
       <c r="J339" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="340">
@@ -10165,13 +10218,15 @@
       <c r="E343" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F343" s="5"/>
+      <c r="F343" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="G343" s="6"/>
       <c r="H343" s="5"/>
       <c r="I343" s="6"/>
       <c r="J343" s="5">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="344">
@@ -10380,7 +10435,9 @@
       <c r="C352" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="D352" s="5"/>
+      <c r="D352" s="3">
+        <v>10000.0</v>
+      </c>
       <c r="E352" s="4"/>
       <c r="F352" s="5"/>
       <c r="G352" s="6"/>
@@ -10388,7 +10445,7 @@
       <c r="I352" s="6"/>
       <c r="J352" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="353">
@@ -10483,6 +10540,43 @@
       <c r="J356" s="5">
         <f t="shared" si="2"/>
         <v>10000</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="2">
+        <v>357.0</v>
+      </c>
+      <c r="B357" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D357" s="3">
+        <v>10000.0</v>
+      </c>
+      <c r="F357" s="3">
+        <v>10000.0</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="2">
+        <v>357.0</v>
+      </c>
+      <c r="B358" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C358" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D358" s="3">
+        <v>10000.0</v>
+      </c>
+      <c r="F358" s="3">
+        <v>10000.0</v>
+      </c>
+      <c r="H358" s="2" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -10491,17 +10585,17 @@
       <sortCondition ref="B1:B1023"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="D2:D356 F2:F356 H2:H356">
+  <conditionalFormatting sqref="D2:D358 F2:F358 H2:H356">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
       <formula>10000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D356 F2:F356 H2:H356">
+  <conditionalFormatting sqref="D2:D358 F2:F358 H2:H356">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
       <formula>5000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D356 F2:F356 H2:H356">
+  <conditionalFormatting sqref="D2:D358 F2:F358 H2:H356">
     <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>

</xml_diff>